<commit_message>
Chasse aux erreurs sur les prix
</commit_message>
<xml_diff>
--- a/Unverified multiformat sources/Exports Nantes 1770.xlsx
+++ b/Unverified multiformat sources/Exports Nantes 1770.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10523"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10709"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/guillaumedaudin/Documents/Recherche/Commerce International Français XVIIIe.xls/Balance du commerce/Retranscriptions_Commerce_France/toflit18_data_GIT/Unverified multiformat sources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B71D3B6-CCB4-404B-8BE9-19C14FAD7098}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8283996B-6D10-0E4C-8EDA-F9B7CC3C3E0E}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="16380" windowHeight="8200" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="36820" windowHeight="32760" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="179017" iterateDelta="1E-4"/>
+  <calcPr calcId="179021" iterateDelta="1E-4"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="ExcelA1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5056" uniqueCount="415">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5057" uniqueCount="416">
   <si>
     <t>numrodeligne</t>
   </si>
@@ -1271,6 +1271,9 @@
   <si>
     <t>probleme</t>
   </si>
+  <si>
+    <t>Erreur de prix dans la source. Je remplace par le prix des exportations pour les îles</t>
+  </si>
 </sst>
 </file>
 
@@ -1896,8 +1899,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AMJ557"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="M1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="W1" sqref="W1"/>
+    <sheetView tabSelected="1" topLeftCell="A91" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="X145" sqref="X145"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -12396,14 +12399,14 @@
       <c r="M145" s="29" t="s">
         <v>40</v>
       </c>
-      <c r="N145" s="30"/>
-      <c r="O145" s="30">
-        <v>1</v>
-      </c>
+      <c r="N145" s="30">
+        <v>14</v>
+      </c>
+      <c r="O145" s="30"/>
       <c r="P145" s="30"/>
       <c r="Q145" s="22">
         <f t="shared" si="15"/>
-        <v>0.05</v>
+        <v>14</v>
       </c>
       <c r="R145" s="31">
         <v>23</v>
@@ -12416,13 +12419,15 @@
       </c>
       <c r="V145" s="25">
         <f t="shared" si="12"/>
-        <v>23</v>
+        <v>6440</v>
       </c>
       <c r="W145" s="26">
         <f t="shared" si="16"/>
-        <v>0</v>
-      </c>
-      <c r="X145" s="29"/>
+        <v>-6417</v>
+      </c>
+      <c r="X145" s="29" t="s">
+        <v>415</v>
+      </c>
       <c r="Y145">
         <v>1</v>
       </c>

</xml_diff>